<commit_message>
Added to desision spreadsheet
</commit_message>
<xml_diff>
--- a/Motor Controller PCB/Desision SpreedSheet.xlsx
+++ b/Motor Controller PCB/Desision SpreedSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Put Ideas here</t>
   </si>
@@ -64,13 +64,37 @@
   </si>
   <si>
     <t>Gate Driver</t>
+  </si>
+  <si>
+    <t>Flyback Diode</t>
+  </si>
+  <si>
+    <t>STPS30M60SG-TR</t>
+  </si>
+  <si>
+    <t>http://www.st.com/content/ccc/resource/technical/document/datasheet/5e/39/b2/48/ff/81/45/23/DM00034932.pdf/files/DM00034932.pdf/jcr:content/translations/en.DM00034932.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/stmicroelectronics/STPS30M60SG-TR/497-12322-1-ND/2826734</t>
+  </si>
+  <si>
+    <t>FSV1045V</t>
+  </si>
+  <si>
+    <t>https://www.fairchildsemi.com/datasheets/FS/FSV1045V.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/fairchild-on-semiconductor/FSV1045V/FSV1045VCT-ND/5255863</t>
+  </si>
+  <si>
+    <t>FSV1045V: Lower voltage drop, cheaper. Cons: 10A Average current; Flyback *shouldn’t* be larger than 7.5A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +138,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -148,27 +180,33 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -454,139 +492,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="6" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="6" width="36.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="9"/>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="8"/>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>4.95</v>
+      </c>
+      <c r="F26">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" ht="36.5" x14ac:dyDescent="0.35">
+      <c r="D27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added Mosfet Network Block
Selected a nMOS to use and added it to the eagle schematic.

Didnt have an eagle part, so I made. I made the pads extra large so we
can get to it with an iron.
</commit_message>
<xml_diff>
--- a/Motor Controller PCB/Desision SpreedSheet.xlsx
+++ b/Motor Controller PCB/Desision SpreedSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Put Ideas here</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>We're going to test the SM74611KTTR. It might fail since its and active diode. It it works, the 28mV forward drop saves a lot of power. Otherwise the FSV1045V is the better option</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/on-semiconductor/NTMFS5C426NT1G/NTMFS5C426NT1GOSCT-ND/6560638</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/products/en?keywords=IRFS7530-7PPbF</t>
+  </si>
+  <si>
+    <t>NTMFS5C426N: Cheaper and better in every way. Package may cause an issue, but I believe I can handle it</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,15 +216,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,7 +238,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -511,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,21 +535,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="11"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="10"/>
       <c r="D2" t="s">
         <v>2</v>
       </c>
@@ -555,32 +567,47 @@
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>6</v>
       </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>4.13</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
@@ -603,17 +630,17 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
@@ -636,29 +663,29 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -666,13 +693,13 @@
       <c r="D24" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -680,13 +707,13 @@
       <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -705,11 +732,11 @@
       </c>
     </row>
     <row r="27" spans="4:7" ht="48.5" x14ac:dyDescent="0.35">
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="10"/>
+      <c r="F27" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -729,8 +756,11 @@
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="G25" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>